<commit_message>
Updated code to run on a per-year or proj_group basis
As a result, there's a tonne more graphs generated.

Also messed with excel a bit more.

Still need to add in grouped bar charts. I thikn instead of trying to do everyhting in one function it will be cleaner to just take the ax from the subplot function and directly use matplotlib.

Co-Authored-By: Rowena-ycj <rowena-ycj@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/skill_analysis_scratch.xlsx
+++ b/skill_analysis_scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\JupyterProj\RowenaIndusProj\rowenaIndustrialReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681E5926-DEB7-407F-8F46-F1CB3ABD3C5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61049EB4-51AB-4A76-9C39-06708038F87E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91381AA0-CDED-4A24-B704-028EFDFCCA12}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="350">
   <si>
     <t>SM1i</t>
   </si>
@@ -1084,6 +1084,9 @@
   </si>
   <si>
     <t>MaxFordham</t>
+  </si>
+  <si>
+    <t>proj_group</t>
   </si>
 </sst>
 </file>
@@ -2163,39 +2166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2204,6 +2174,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -2220,19 +2193,42 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2557,6 +2553,13 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3737,7 +3740,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{874454D2-E7A1-49C7-B3D6-F4649E047457}" name="Table1" displayName="Table1" ref="E4:J46" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{874454D2-E7A1-49C7-B3D6-F4649E047457}" name="Table1" displayName="Table1" ref="E4:J46" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
   <autoFilter ref="E4:J46" xr:uid="{FEDCF0A9-C11D-4890-955E-26CD106F3055}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3747,19 +3750,19 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{940E411E-8400-40B8-96F9-44DFEFD8B182}" name="Project Name" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{940E411E-8400-40B8-96F9-44DFEFD8B182}" name="Project Name" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{BDE580CA-F9F8-4D94-9E58-6003AEF4AA73}" name="Sector"/>
-    <tableColumn id="3" xr3:uid="{546043E9-4585-40C9-947B-FB0ACAAF1C1C}" name="RIBA Stage" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{546043E9-4585-40C9-947B-FB0ACAAF1C1C}" name="RIBA Stage" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{76BAC2BF-66A2-4DE3-9C84-B30533F75941}" name="Responsibilites"/>
     <tableColumn id="5" xr3:uid="{FAC3E5BE-A627-47EF-842A-936B8C5C24E4}" name="Technical Level"/>
-    <tableColumn id="6" xr3:uid="{3C424575-28AB-4F48-860E-C6F0286F864B}" name="Technical Background" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{3C424575-28AB-4F48-860E-C6F0286F864B}" name="Technical Background" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB18F5F7-94C3-412F-B41C-89A49D3A1B6E}" name="Table2" displayName="Table2" ref="E4:H14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB18F5F7-94C3-412F-B41C-89A49D3A1B6E}" name="Table2" displayName="Table2" ref="E4:H14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="E4:H14" xr:uid="{AA3D3DA4-2083-490B-A96B-2B6A8C8A062C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3767,17 +3770,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D8A65525-04C8-4BE8-8B00-98640AF74A25}" name="Date" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B8AB7846-FFD4-480C-9E95-269BFDB4D83F}" name="Type" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{ACD4220A-1F09-4CA6-83C8-1ADE750BFEDF}" name="Organisation" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{14F76FFF-750E-4CE0-B5B1-C105AAD8B551}" name="Title" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{D8A65525-04C8-4BE8-8B00-98640AF74A25}" name="Date" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B8AB7846-FFD4-480C-9E95-269BFDB4D83F}" name="Type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{ACD4220A-1F09-4CA6-83C8-1ADE750BFEDF}" name="Organisation" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{14F76FFF-750E-4CE0-B5B1-C105AAD8B551}" name="Title" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99DCEDA8-FD6A-4E18-9BB2-84664FBDA263}" name="Table3" displayName="Table3" ref="E4:H23" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99DCEDA8-FD6A-4E18-9BB2-84664FBDA263}" name="Table3" displayName="Table3" ref="E4:H23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="E4:H23" xr:uid="{E199B8BB-BC91-441E-9101-4AE76CC62D13}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3785,10 +3788,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{590C04C5-5CDC-4ECD-B6EA-7E8890540C41}" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{3498CE5B-8610-4066-A61D-90644C3BD461}" name="Type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{2AD8B7EA-1272-40CF-AABF-BACD4051D629}" name="Title" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{3D9453BF-042C-4CB9-B176-9466A2A70913}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{590C04C5-5CDC-4ECD-B6EA-7E8890540C41}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3498CE5B-8610-4066-A61D-90644C3BD461}" name="Type" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2AD8B7EA-1272-40CF-AABF-BACD4051D629}" name="Title" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{3D9453BF-042C-4CB9-B176-9466A2A70913}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4096,7 +4099,7 @@
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C2" sqref="C2"/>
-      <selection pane="bottomLeft" activeCell="AZ7" sqref="AZ7"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4289,68 +4292,70 @@
     <row r="3" spans="1:78" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="199" t="s">
+      <c r="C3" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D3" s="209" t="s">
         <v>343</v>
       </c>
-      <c r="E3" s="199"/>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="199"/>
-      <c r="I3" s="199"/>
-      <c r="J3" s="199"/>
-      <c r="K3" s="199"/>
-      <c r="L3" s="195" t="s">
+      <c r="E3" s="209"/>
+      <c r="F3" s="209"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="209"/>
+      <c r="J3" s="209"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="206" t="s">
         <v>344</v>
       </c>
-      <c r="M3" s="195"/>
-      <c r="N3" s="195"/>
-      <c r="O3" s="195"/>
-      <c r="P3" s="195"/>
-      <c r="Q3" s="195"/>
-      <c r="R3" s="195"/>
-      <c r="S3" s="195"/>
-      <c r="T3" s="196" t="s">
+      <c r="M3" s="206"/>
+      <c r="N3" s="206"/>
+      <c r="O3" s="206"/>
+      <c r="P3" s="206"/>
+      <c r="Q3" s="206"/>
+      <c r="R3" s="206"/>
+      <c r="S3" s="206"/>
+      <c r="T3" s="207" t="s">
         <v>345</v>
       </c>
-      <c r="U3" s="196"/>
-      <c r="V3" s="196"/>
-      <c r="W3" s="196"/>
-      <c r="X3" s="196"/>
-      <c r="Y3" s="196"/>
-      <c r="Z3" s="196"/>
-      <c r="AA3" s="196"/>
-      <c r="AB3" s="197" t="s">
+      <c r="U3" s="207"/>
+      <c r="V3" s="207"/>
+      <c r="W3" s="207"/>
+      <c r="X3" s="207"/>
+      <c r="Y3" s="207"/>
+      <c r="Z3" s="207"/>
+      <c r="AA3" s="207"/>
+      <c r="AB3" s="208" t="s">
         <v>346</v>
       </c>
-      <c r="AC3" s="197"/>
-      <c r="AD3" s="197"/>
-      <c r="AE3" s="197"/>
-      <c r="AF3" s="197"/>
-      <c r="AG3" s="206" t="s">
+      <c r="AC3" s="208"/>
+      <c r="AD3" s="208"/>
+      <c r="AE3" s="208"/>
+      <c r="AF3" s="208"/>
+      <c r="AG3" s="196" t="s">
         <v>347</v>
       </c>
-      <c r="AH3" s="206"/>
-      <c r="AI3" s="206"/>
-      <c r="AJ3" s="206"/>
-      <c r="AK3" s="206"/>
-      <c r="AL3" s="206"/>
-      <c r="AM3" s="206"/>
-      <c r="AN3" s="207" t="s">
+      <c r="AH3" s="196"/>
+      <c r="AI3" s="196"/>
+      <c r="AJ3" s="196"/>
+      <c r="AK3" s="196"/>
+      <c r="AL3" s="196"/>
+      <c r="AM3" s="196"/>
+      <c r="AN3" s="197" t="s">
         <v>348</v>
       </c>
-      <c r="AO3" s="208"/>
-      <c r="AP3" s="208"/>
-      <c r="AQ3" s="208"/>
-      <c r="AR3" s="208"/>
-      <c r="AS3" s="208"/>
-      <c r="AT3" s="209"/>
-      <c r="AU3" s="202" t="s">
+      <c r="AO3" s="198"/>
+      <c r="AP3" s="198"/>
+      <c r="AQ3" s="198"/>
+      <c r="AR3" s="198"/>
+      <c r="AS3" s="198"/>
+      <c r="AT3" s="199"/>
+      <c r="AU3" s="191" t="s">
         <v>166</v>
       </c>
-      <c r="AV3" s="203"/>
-      <c r="AW3" s="203"/>
-      <c r="AX3" s="204"/>
+      <c r="AV3" s="192"/>
+      <c r="AW3" s="192"/>
+      <c r="AX3" s="193"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
@@ -4381,10 +4386,10 @@
       <c r="BZ3" s="4"/>
     </row>
     <row r="4" spans="1:78" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="191" t="s">
+      <c r="A4" s="203" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="198" t="s">
+      <c r="B4" s="201" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -4503,8 +4508,8 @@
       <c r="BH4" s="38"/>
     </row>
     <row r="5" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A5" s="192"/>
-      <c r="B5" s="198"/>
+      <c r="A5" s="204"/>
+      <c r="B5" s="201"/>
       <c r="C5" s="12" t="s">
         <v>1</v>
       </c>
@@ -4603,8 +4608,8 @@
       <c r="BH5" s="38"/>
     </row>
     <row r="6" spans="1:78" ht="116.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="192"/>
-      <c r="B6" s="198"/>
+      <c r="A6" s="204"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="39" t="s">
         <v>2</v>
       </c>
@@ -4675,8 +4680,8 @@
       <c r="BH6" s="44"/>
     </row>
     <row r="7" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A7" s="192"/>
-      <c r="B7" s="198" t="s">
+      <c r="A7" s="204"/>
+      <c r="B7" s="201" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -4789,8 +4794,8 @@
       <c r="BH7" s="47"/>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A8" s="192"/>
-      <c r="B8" s="198"/>
+      <c r="A8" s="204"/>
+      <c r="B8" s="201"/>
       <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
@@ -4879,8 +4884,8 @@
       <c r="BH8" s="38"/>
     </row>
     <row r="9" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A9" s="192"/>
-      <c r="B9" s="198"/>
+      <c r="A9" s="204"/>
+      <c r="B9" s="201"/>
       <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
@@ -4951,8 +4956,8 @@
       <c r="BH9" s="44"/>
     </row>
     <row r="10" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A10" s="192"/>
-      <c r="B10" s="198" t="s">
+      <c r="A10" s="204"/>
+      <c r="B10" s="201" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -5041,8 +5046,8 @@
       <c r="BH10" s="47"/>
     </row>
     <row r="11" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A11" s="192"/>
-      <c r="B11" s="198"/>
+      <c r="A11" s="204"/>
+      <c r="B11" s="201"/>
       <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
@@ -5117,7 +5122,7 @@
       <c r="BH11" s="44"/>
     </row>
     <row r="12" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A12" s="192"/>
+      <c r="A12" s="204"/>
       <c r="B12" s="14" t="s">
         <v>14</v>
       </c>
@@ -5217,7 +5222,7 @@
       <c r="BH12" s="53"/>
     </row>
     <row r="13" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A13" s="192"/>
+      <c r="A13" s="204"/>
       <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
@@ -5291,7 +5296,7 @@
       <c r="BH13" s="53"/>
     </row>
     <row r="14" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A14" s="193"/>
+      <c r="A14" s="205"/>
       <c r="B14" s="14" t="s">
         <v>16</v>
       </c>
@@ -5395,7 +5400,7 @@
       <c r="BH14" s="53"/>
     </row>
     <row r="15" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="200" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="194" t="s">
@@ -5477,7 +5482,7 @@
       <c r="BH15" s="47"/>
     </row>
     <row r="16" spans="1:78" x14ac:dyDescent="0.3">
-      <c r="A16" s="201"/>
+      <c r="A16" s="200"/>
       <c r="B16" s="194"/>
       <c r="C16" s="12" t="s">
         <v>19</v>
@@ -5573,7 +5578,7 @@
       <c r="BH16" s="38"/>
     </row>
     <row r="17" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A17" s="201"/>
+      <c r="A17" s="200"/>
       <c r="B17" s="194"/>
       <c r="C17" s="12" t="s">
         <v>20</v>
@@ -5647,8 +5652,8 @@
       <c r="BH17" s="44"/>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A18" s="201"/>
-      <c r="B18" s="200" t="s">
+      <c r="A18" s="200"/>
+      <c r="B18" s="202" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -5729,8 +5734,8 @@
       <c r="BH18" s="47"/>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A19" s="201"/>
-      <c r="B19" s="200"/>
+      <c r="A19" s="200"/>
+      <c r="B19" s="202"/>
       <c r="C19" s="12" t="s">
         <v>22</v>
       </c>
@@ -5803,8 +5808,8 @@
       <c r="BH19" s="44"/>
     </row>
     <row r="20" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A20" s="201"/>
-      <c r="B20" s="198" t="s">
+      <c r="A20" s="200"/>
+      <c r="B20" s="201" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -5891,8 +5896,8 @@
       <c r="BH20" s="47"/>
     </row>
     <row r="21" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A21" s="201"/>
-      <c r="B21" s="198"/>
+      <c r="A21" s="200"/>
+      <c r="B21" s="201"/>
       <c r="C21" s="12" t="s">
         <v>24</v>
       </c>
@@ -5969,8 +5974,8 @@
       <c r="BH21" s="38"/>
     </row>
     <row r="22" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A22" s="201"/>
-      <c r="B22" s="198"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="201"/>
       <c r="C22" s="12" t="s">
         <v>25</v>
       </c>
@@ -6041,8 +6046,8 @@
       <c r="BH22" s="44"/>
     </row>
     <row r="23" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A23" s="201"/>
-      <c r="B23" s="198" t="s">
+      <c r="A23" s="200"/>
+      <c r="B23" s="201" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -6127,8 +6132,8 @@
       <c r="BH23" s="47"/>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A24" s="201"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
       <c r="C24" s="12" t="s">
         <v>27</v>
       </c>
@@ -6203,8 +6208,8 @@
       <c r="BH24" s="38"/>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A25" s="201"/>
-      <c r="B25" s="198"/>
+      <c r="A25" s="200"/>
+      <c r="B25" s="201"/>
       <c r="C25" s="12" t="s">
         <v>28</v>
       </c>
@@ -6273,7 +6278,7 @@
       <c r="BH25" s="44"/>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A26" s="201"/>
+      <c r="A26" s="200"/>
       <c r="B26" s="15" t="s">
         <v>34</v>
       </c>
@@ -6359,7 +6364,7 @@
       <c r="BH26" s="53"/>
     </row>
     <row r="27" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A27" s="201"/>
+      <c r="A27" s="200"/>
       <c r="B27" s="15" t="s">
         <v>35</v>
       </c>
@@ -6441,10 +6446,10 @@
       <c r="BH27" s="53"/>
     </row>
     <row r="28" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A28" s="201" t="s">
+      <c r="A28" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="198" t="s">
+      <c r="B28" s="201" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -6541,8 +6546,8 @@
       <c r="BH28" s="47"/>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A29" s="201"/>
-      <c r="B29" s="198"/>
+      <c r="A29" s="200"/>
+      <c r="B29" s="201"/>
       <c r="C29" s="12" t="s">
         <v>38</v>
       </c>
@@ -6611,8 +6616,8 @@
       <c r="BH29" s="44"/>
     </row>
     <row r="30" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A30" s="201"/>
-      <c r="B30" s="198" t="s">
+      <c r="A30" s="200"/>
+      <c r="B30" s="201" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -6705,8 +6710,8 @@
       <c r="BH30" s="47"/>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A31" s="201"/>
-      <c r="B31" s="198"/>
+      <c r="A31" s="200"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="12" t="s">
         <v>40</v>
       </c>
@@ -6783,8 +6788,8 @@
       <c r="BH31" s="44"/>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A32" s="201"/>
-      <c r="B32" s="198" t="s">
+      <c r="A32" s="200"/>
+      <c r="B32" s="201" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -6863,8 +6868,8 @@
       <c r="BH32" s="47"/>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A33" s="201"/>
-      <c r="B33" s="198"/>
+      <c r="A33" s="200"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="12" t="s">
         <v>42</v>
       </c>
@@ -6929,8 +6934,8 @@
       <c r="BH33" s="38"/>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A34" s="201"/>
-      <c r="B34" s="198"/>
+      <c r="A34" s="200"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="12" t="s">
         <v>43</v>
       </c>
@@ -6993,8 +6998,8 @@
       <c r="BH34" s="44"/>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A35" s="201"/>
-      <c r="B35" s="198" t="s">
+      <c r="A35" s="200"/>
+      <c r="B35" s="201" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -7085,8 +7090,8 @@
       <c r="BH35" s="47"/>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A36" s="201"/>
-      <c r="B36" s="198"/>
+      <c r="A36" s="200"/>
+      <c r="B36" s="201"/>
       <c r="C36" s="12" t="s">
         <v>45</v>
       </c>
@@ -7155,8 +7160,8 @@
       <c r="BH36" s="44"/>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A37" s="201"/>
-      <c r="B37" s="198" t="s">
+      <c r="A37" s="200"/>
+      <c r="B37" s="201" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="12" t="s">
@@ -7229,8 +7234,8 @@
       <c r="BH37" s="47"/>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A38" s="201"/>
-      <c r="B38" s="198"/>
+      <c r="A38" s="200"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="12" t="s">
         <v>47</v>
       </c>
@@ -7295,7 +7300,7 @@
       <c r="BH38" s="44"/>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A39" s="201"/>
+      <c r="A39" s="200"/>
       <c r="B39" s="15" t="s">
         <v>48</v>
       </c>
@@ -7379,7 +7384,7 @@
       <c r="BH39" s="53"/>
     </row>
     <row r="40" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A40" s="201"/>
+      <c r="A40" s="200"/>
       <c r="B40" s="15" t="s">
         <v>51</v>
       </c>
@@ -7457,7 +7462,7 @@
       <c r="BH40" s="53"/>
     </row>
     <row r="41" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A41" s="201"/>
+      <c r="A41" s="200"/>
       <c r="B41" s="15" t="s">
         <v>52</v>
       </c>
@@ -7535,10 +7540,10 @@
       <c r="BH41" s="53"/>
     </row>
     <row r="42" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A42" s="201" t="s">
+      <c r="A42" s="200" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="198" t="s">
+      <c r="B42" s="201" t="s">
         <v>54</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -7623,8 +7628,8 @@
       <c r="BH42" s="47"/>
     </row>
     <row r="43" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A43" s="201"/>
-      <c r="B43" s="198"/>
+      <c r="A43" s="200"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="12" t="s">
         <v>55</v>
       </c>
@@ -7707,7 +7712,7 @@
       <c r="BH43" s="44"/>
     </row>
     <row r="44" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A44" s="201"/>
+      <c r="A44" s="200"/>
       <c r="B44" s="15" t="s">
         <v>56</v>
       </c>
@@ -7789,7 +7794,7 @@
       <c r="BH44" s="53"/>
     </row>
     <row r="45" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A45" s="201"/>
+      <c r="A45" s="200"/>
       <c r="B45" s="194" t="s">
         <v>67</v>
       </c>
@@ -7873,7 +7878,7 @@
       <c r="BH45" s="47"/>
     </row>
     <row r="46" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A46" s="201"/>
+      <c r="A46" s="200"/>
       <c r="B46" s="194"/>
       <c r="C46" s="12" t="s">
         <v>58</v>
@@ -7943,7 +7948,7 @@
       <c r="BH46" s="38"/>
     </row>
     <row r="47" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A47" s="201"/>
+      <c r="A47" s="200"/>
       <c r="B47" s="194"/>
       <c r="C47" s="12" t="s">
         <v>59</v>
@@ -8007,7 +8012,7 @@
       <c r="BH47" s="44"/>
     </row>
     <row r="48" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A48" s="201"/>
+      <c r="A48" s="200"/>
       <c r="B48" s="194" t="s">
         <v>68</v>
       </c>
@@ -8109,7 +8114,7 @@
       <c r="BH48" s="47"/>
     </row>
     <row r="49" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A49" s="201"/>
+      <c r="A49" s="200"/>
       <c r="B49" s="194"/>
       <c r="C49" s="12" t="s">
         <v>61</v>
@@ -8187,7 +8192,7 @@
       <c r="BH49" s="44"/>
     </row>
     <row r="50" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A50" s="201"/>
+      <c r="A50" s="200"/>
       <c r="B50" s="194" t="s">
         <v>62</v>
       </c>
@@ -8273,7 +8278,7 @@
       <c r="BH50" s="47"/>
     </row>
     <row r="51" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A51" s="201"/>
+      <c r="A51" s="200"/>
       <c r="B51" s="194"/>
       <c r="C51" s="12" t="s">
         <v>63</v>
@@ -8349,7 +8354,7 @@
       <c r="BH51" s="44"/>
     </row>
     <row r="52" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A52" s="201"/>
+      <c r="A52" s="200"/>
       <c r="B52" s="194" t="s">
         <v>69</v>
       </c>
@@ -8439,7 +8444,7 @@
       <c r="BH52" s="47"/>
     </row>
     <row r="53" spans="1:60" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="201"/>
+      <c r="A53" s="200"/>
       <c r="B53" s="194"/>
       <c r="C53" s="12" t="s">
         <v>148</v>
@@ -8513,7 +8518,7 @@
       <c r="BH53" s="38"/>
     </row>
     <row r="54" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A54" s="201"/>
+      <c r="A54" s="200"/>
       <c r="B54" s="194"/>
       <c r="C54" s="12" t="s">
         <v>65</v>
@@ -8577,7 +8582,7 @@
       <c r="BH54" s="44"/>
     </row>
     <row r="55" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A55" s="201"/>
+      <c r="A55" s="200"/>
       <c r="B55" s="14" t="s">
         <v>70</v>
       </c>
@@ -8651,7 +8656,7 @@
       <c r="BH55" s="53"/>
     </row>
     <row r="56" spans="1:60" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="201" t="s">
+      <c r="A56" s="200" t="s">
         <v>97</v>
       </c>
       <c r="B56" s="194" t="s">
@@ -8761,7 +8766,7 @@
       <c r="BH56" s="47"/>
     </row>
     <row r="57" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A57" s="201"/>
+      <c r="A57" s="200"/>
       <c r="B57" s="194"/>
       <c r="C57" s="12" t="s">
         <v>73</v>
@@ -8857,7 +8862,7 @@
       <c r="BH57" s="44"/>
     </row>
     <row r="58" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A58" s="201"/>
+      <c r="A58" s="200"/>
       <c r="B58" s="194" t="s">
         <v>91</v>
       </c>
@@ -8959,7 +8964,7 @@
       <c r="BH58" s="47"/>
     </row>
     <row r="59" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A59" s="201"/>
+      <c r="A59" s="200"/>
       <c r="B59" s="194"/>
       <c r="C59" s="12" t="s">
         <v>75</v>
@@ -9043,7 +9048,7 @@
       <c r="BH59" s="38"/>
     </row>
     <row r="60" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A60" s="201"/>
+      <c r="A60" s="200"/>
       <c r="B60" s="194"/>
       <c r="C60" s="12" t="s">
         <v>76</v>
@@ -9107,7 +9112,7 @@
       <c r="BH60" s="44"/>
     </row>
     <row r="61" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A61" s="201"/>
+      <c r="A61" s="200"/>
       <c r="B61" s="194" t="s">
         <v>92</v>
       </c>
@@ -9189,7 +9194,7 @@
       <c r="BH61" s="47"/>
     </row>
     <row r="62" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A62" s="201"/>
+      <c r="A62" s="200"/>
       <c r="B62" s="194"/>
       <c r="C62" s="12" t="s">
         <v>149</v>
@@ -9265,7 +9270,7 @@
       <c r="BH62" s="44"/>
     </row>
     <row r="63" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A63" s="201"/>
+      <c r="A63" s="200"/>
       <c r="B63" s="194" t="s">
         <v>93</v>
       </c>
@@ -9365,7 +9370,7 @@
       <c r="BH63" s="47"/>
     </row>
     <row r="64" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A64" s="201"/>
+      <c r="A64" s="200"/>
       <c r="B64" s="194"/>
       <c r="C64" s="12" t="s">
         <v>93</v>
@@ -9447,7 +9452,7 @@
       <c r="BH64" s="38"/>
     </row>
     <row r="65" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A65" s="201"/>
+      <c r="A65" s="200"/>
       <c r="B65" s="194"/>
       <c r="C65" s="135" t="s">
         <v>79</v>
@@ -9529,7 +9534,7 @@
       <c r="BH65" s="44"/>
     </row>
     <row r="66" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A66" s="201"/>
+      <c r="A66" s="200"/>
       <c r="B66" s="14" t="s">
         <v>80</v>
       </c>
@@ -9607,7 +9612,7 @@
       <c r="BH66" s="53"/>
     </row>
     <row r="67" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A67" s="201"/>
+      <c r="A67" s="200"/>
       <c r="B67" s="194" t="s">
         <v>94</v>
       </c>
@@ -9699,7 +9704,7 @@
       <c r="BH67" s="47"/>
     </row>
     <row r="68" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A68" s="201"/>
+      <c r="A68" s="200"/>
       <c r="B68" s="194"/>
       <c r="C68" s="12" t="s">
         <v>82</v>
@@ -9775,7 +9780,7 @@
       <c r="BH68" s="44"/>
     </row>
     <row r="69" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A69" s="201"/>
+      <c r="A69" s="200"/>
       <c r="B69" s="14" t="s">
         <v>83</v>
       </c>
@@ -9853,7 +9858,7 @@
       <c r="BH69" s="53"/>
     </row>
     <row r="70" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A70" s="201"/>
+      <c r="A70" s="200"/>
       <c r="B70" s="14" t="s">
         <v>84</v>
       </c>
@@ -9939,7 +9944,7 @@
       <c r="BH70" s="53"/>
     </row>
     <row r="71" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A71" s="201"/>
+      <c r="A71" s="200"/>
       <c r="B71" s="14" t="s">
         <v>95</v>
       </c>
@@ -10021,7 +10026,7 @@
       <c r="BH71" s="53"/>
     </row>
     <row r="72" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A72" s="201"/>
+      <c r="A72" s="200"/>
       <c r="B72" s="14" t="s">
         <v>96</v>
       </c>
@@ -10097,7 +10102,7 @@
       <c r="BH72" s="53"/>
     </row>
     <row r="73" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A73" s="201"/>
+      <c r="A73" s="200"/>
       <c r="B73" s="194" t="s">
         <v>87</v>
       </c>
@@ -10179,7 +10184,7 @@
       <c r="BH73" s="47"/>
     </row>
     <row r="74" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A74" s="201"/>
+      <c r="A74" s="200"/>
       <c r="B74" s="194"/>
       <c r="C74" s="12" t="s">
         <v>87</v>
@@ -10257,7 +10262,7 @@
       <c r="BH74" s="38"/>
     </row>
     <row r="75" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A75" s="201"/>
+      <c r="A75" s="200"/>
       <c r="B75" s="194"/>
       <c r="C75" s="12" t="s">
         <v>89</v>
@@ -10333,7 +10338,7 @@
       <c r="BH75" s="44"/>
     </row>
     <row r="76" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A76" s="205" t="s">
+      <c r="A76" s="195" t="s">
         <v>106</v>
       </c>
       <c r="B76" s="14" t="s">
@@ -10443,7 +10448,7 @@
       <c r="BH76" s="53"/>
     </row>
     <row r="77" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A77" s="205"/>
+      <c r="A77" s="195"/>
       <c r="B77" s="14" t="s">
         <v>99</v>
       </c>
@@ -10537,7 +10542,7 @@
       <c r="BH77" s="53"/>
     </row>
     <row r="78" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A78" s="205"/>
+      <c r="A78" s="195"/>
       <c r="B78" s="194" t="s">
         <v>105</v>
       </c>
@@ -10655,7 +10660,7 @@
       <c r="BH78" s="47"/>
     </row>
     <row r="79" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A79" s="205"/>
+      <c r="A79" s="195"/>
       <c r="B79" s="194"/>
       <c r="C79" s="12" t="s">
         <v>102</v>
@@ -10759,7 +10764,7 @@
       <c r="BH79" s="38"/>
     </row>
     <row r="80" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A80" s="205"/>
+      <c r="A80" s="195"/>
       <c r="B80" s="194"/>
       <c r="C80" s="12" t="s">
         <v>103</v>
@@ -10833,7 +10838,7 @@
       <c r="BH80" s="44"/>
     </row>
     <row r="81" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A81" s="205"/>
+      <c r="A81" s="195"/>
       <c r="B81" s="194" t="s">
         <v>104</v>
       </c>
@@ -10931,7 +10936,7 @@
       <c r="BH81" s="47"/>
     </row>
     <row r="82" spans="1:60" x14ac:dyDescent="0.3">
-      <c r="A82" s="205"/>
+      <c r="A82" s="195"/>
       <c r="B82" s="194"/>
       <c r="C82" s="12" t="s">
         <v>104</v>
@@ -11017,6 +11022,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="L3:S3"/>
+    <mergeCell ref="T3:AA3"/>
+    <mergeCell ref="AB3:AF3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A15:A27"/>
+    <mergeCell ref="A4:A14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A42:A55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A28:A41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="AU3:AX3"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B81:B82"/>
@@ -11033,28 +11060,6 @@
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A42:A55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A28:A41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A15:A27"/>
-    <mergeCell ref="A4:A14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="L3:S3"/>
-    <mergeCell ref="T3:AA3"/>
-    <mergeCell ref="AB3:AF3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D3:K3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="D4:AX14">
@@ -11118,7 +11123,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:AX54 D56:AX82 D55:AM55 AO55:AX55">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12895,18 +12900,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13081,14 +13086,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6EE32A0-71F8-4E54-BFDA-6902525DD513}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3192F1-D77C-4218-9B8F-6C8BC205D392}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -13101,6 +13098,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6EE32A0-71F8-4E54-BFDA-6902525DD513}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>